<commit_message>
fix: wrong color in colum
</commit_message>
<xml_diff>
--- a/.design/Join_Projektuebersicht.xlsx
+++ b/.design/Join_Projektuebersicht.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470D80F3-9A00-49AF-B9AE-2B9A2241A1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="2" name="Folder and File" state="visible" r:id="rId4"/>
-    <sheet sheetId="3" name="DummyData" state="visible" r:id="rId5"/>
+    <sheet name="Folder and File" sheetId="2" r:id="rId1"/>
+    <sheet name="DummyData" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -394,10 +395,10 @@
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
         <color theme="1"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (für Login/Registrierung bzw. Profil)</t>
     </r>
@@ -406,7 +407,7 @@
     <t>// users (Collection)</t>
   </si>
   <si>
-    <t xml:space="preserve">Kann sich einloggen
+    <t>Kann sich einloggen
 Sieht Summary, Board, Contacts
 Erstellt, bearbeitet und verschiebt Tasks</t>
   </si>
@@ -464,10 +465,10 @@
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
         <color theme="1"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (für Zuweisungen)</t>
     </r>
@@ -476,7 +477,7 @@
     <t>// contacts (Collection)</t>
   </si>
   <si>
-    <t xml:space="preserve">Können Tasks zugewiesen bekommen
+    <t>Können Tasks zugewiesen bekommen
 Müssen keinen Login haben
 Dienen rein der Organisation</t>
   </si>
@@ -528,10 +529,10 @@
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
         <color theme="1"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (fürs Board)</t>
     </r>
@@ -663,38 +664,38 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color theme="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
-      <sz val="10"/>
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
@@ -765,7 +766,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1095,26 +1096,26 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
-    <col min="5" max="5" width="19.25" customWidth="1"/>
-    <col min="6" max="6" width="38.875" customWidth="1"/>
-    <col min="7" max="7" width="13.875" customWidth="1"/>
-    <col min="8" max="8" width="71.25" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="71.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" ht="15.75" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1"/>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1140,7 +1141,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -1158,7 +1159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -1176,7 +1177,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
@@ -1194,7 +1195,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1212,7 +1213,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1230,7 +1231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1248,7 +1249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" ht="29.25" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="29.25" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1268,7 +1269,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1286,7 +1287,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1304,7 +1305,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1322,7 +1323,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3" t="s">
@@ -1340,7 +1341,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1358,7 +1359,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1376,7 +1377,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1394,7 +1395,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1412,11 +1413,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E20" s="2"/>
@@ -1430,7 +1431,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1448,7 +1449,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" ht="29.25" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="29.25" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1466,7 +1467,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3" t="s">
@@ -1484,7 +1485,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1502,7 +1503,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1520,7 +1521,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1538,7 +1539,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1556,7 +1557,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15" customHeight="1">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1574,7 +1575,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1592,7 +1593,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1610,7 +1611,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1628,7 +1629,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3" t="s">
@@ -1646,7 +1647,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1664,7 +1665,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1682,7 +1683,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1700,7 +1701,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1718,7 +1719,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15" customHeight="1">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1736,7 +1737,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1754,7 +1755,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1772,7 +1773,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1790,7 +1791,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1810,31 +1811,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1"/>
-    <hyperlink ref="H11" r:id="rId2"/>
-    <hyperlink ref="H24" r:id="rId3"/>
-    <hyperlink ref="H28" r:id="rId4"/>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:C97"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.625" customWidth="1"/>
-    <col min="2" max="2" width="59.625" customWidth="1"/>
-    <col min="3" max="3" width="36.125" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="59.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="42.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="42.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>124</v>
       </c>
@@ -1845,37 +1846,37 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15">
       <c r="B3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15">
       <c r="B4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15">
       <c r="B5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15">
       <c r="B6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15">
       <c r="B7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15">
       <c r="B8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15">
       <c r="B9" t="s">
         <v>133</v>
       </c>
@@ -1883,52 +1884,52 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15">
       <c r="B10" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15">
       <c r="B11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15">
       <c r="B12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15">
       <c r="B13" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15">
       <c r="B14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15">
       <c r="B15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15">
       <c r="B16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15">
       <c r="B17" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15">
       <c r="B18" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="21" ht="42.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="42.75" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>143</v>
       </c>
@@ -1939,122 +1940,122 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15">
       <c r="B22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15">
       <c r="B23" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15">
       <c r="B24" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15">
       <c r="B25" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15">
       <c r="B26" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15">
       <c r="B27" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15">
       <c r="B28" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15">
       <c r="B29" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15">
       <c r="B30" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15">
       <c r="B31" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15">
       <c r="B32" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="15">
       <c r="B33" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="15">
       <c r="B34" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="15">
       <c r="B35" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="15">
       <c r="B36" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="15">
       <c r="B37" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="15">
       <c r="B38" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="15">
       <c r="B39" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="15">
       <c r="B40" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="15">
       <c r="B41" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="15">
       <c r="B42" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="15">
       <c r="B43" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="15">
       <c r="B44" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="15">
       <c r="A47" s="5" t="s">
         <v>160</v>
       </c>
@@ -2062,37 +2063,37 @@
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="15">
       <c r="B48" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" ht="15">
       <c r="B49" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" ht="15">
       <c r="B50" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" ht="15">
       <c r="B51" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" ht="15">
       <c r="B52" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" ht="15">
       <c r="B53" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" ht="15">
       <c r="B54" t="s">
         <v>166</v>
       </c>
@@ -2100,7 +2101,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" ht="15">
       <c r="B55" t="s">
         <v>168</v>
       </c>
@@ -2108,7 +2109,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" ht="15">
       <c r="B56" t="s">
         <v>170</v>
       </c>
@@ -2116,212 +2117,212 @@
         <v>171</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" ht="15">
       <c r="B57" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" ht="15">
       <c r="B58" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" ht="15">
       <c r="B59" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" ht="15">
       <c r="B60" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" ht="15">
       <c r="B61" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" ht="15">
       <c r="B62" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" ht="15">
       <c r="B63" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" ht="15">
       <c r="B64" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" ht="15">
       <c r="B65" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" ht="15">
       <c r="B66" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" ht="15">
       <c r="B67" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" ht="15">
       <c r="B68" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" ht="15">
       <c r="B69" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" ht="15">
       <c r="B70" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" ht="15">
       <c r="B71" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" ht="15">
       <c r="B72" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" ht="15">
       <c r="B73" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" ht="15">
       <c r="B74" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" ht="15">
       <c r="B75" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" ht="15">
       <c r="B76" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" ht="15">
       <c r="B77" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" ht="15">
       <c r="B78" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" ht="15">
       <c r="B79" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" ht="15">
       <c r="B80" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" ht="15">
       <c r="B81" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" ht="15">
       <c r="B82" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" ht="15">
       <c r="B83" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" ht="15">
       <c r="B84" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" ht="15">
       <c r="B85" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" ht="15">
       <c r="B86" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" ht="15">
       <c r="B87" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" ht="15">
       <c r="B88" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" ht="15">
       <c r="B89" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" ht="15">
       <c r="B90" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" ht="15">
       <c r="B91" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" ht="15">
       <c r="B92" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" ht="15">
       <c r="B93" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" ht="15">
       <c r="B94" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" ht="15">
       <c r="B95" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" ht="15">
       <c r="B96" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" ht="15">
       <c r="B97" t="s">
         <v>142</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: work for Fernando
</commit_message>
<xml_diff>
--- a/.design/Join_Projektuebersicht.xlsx
+++ b/.design/Join_Projektuebersicht.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470D80F3-9A00-49AF-B9AE-2B9A2241A1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295"/>
   </bookViews>
   <sheets>
-    <sheet name="Folder and File" sheetId="2" r:id="rId1"/>
-    <sheet name="DummyData" sheetId="3" r:id="rId2"/>
+    <sheet sheetId="2" name="Folder and File" state="visible" r:id="rId4"/>
+    <sheet sheetId="3" name="DummyData" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="203">
   <si>
     <t>Name/Namen</t>
   </si>
@@ -70,6 +69,9 @@
   </si>
   <si>
     <t>Alle inhaltlichen Seiten (Views).</t>
+  </si>
+  <si>
+    <t>Fernando</t>
   </si>
   <si>
     <t>login.html</t>
@@ -395,10 +397,10 @@
     </r>
     <r>
       <rPr>
+        <color theme="1"/>
+        <family val="2"/>
         <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (für Login/Registrierung bzw. Profil)</t>
     </r>
@@ -407,7 +409,7 @@
     <t>// users (Collection)</t>
   </si>
   <si>
-    <t>Kann sich einloggen
+    <t xml:space="preserve">Kann sich einloggen
 Sieht Summary, Board, Contacts
 Erstellt, bearbeitet und verschiebt Tasks</t>
   </si>
@@ -465,10 +467,10 @@
     </r>
     <r>
       <rPr>
+        <color theme="1"/>
+        <family val="2"/>
         <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (für Zuweisungen)</t>
     </r>
@@ -477,7 +479,7 @@
     <t>// contacts (Collection)</t>
   </si>
   <si>
-    <t>Können Tasks zugewiesen bekommen
+    <t xml:space="preserve">Können Tasks zugewiesen bekommen
 Müssen keinen Login haben
 Dienen rein der Organisation</t>
   </si>
@@ -529,10 +531,10 @@
     </r>
     <r>
       <rPr>
+        <color theme="1"/>
+        <family val="2"/>
         <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (fürs Board)</t>
     </r>
@@ -664,38 +666,38 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <color theme="1"/>
+      <family val="2"/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
+      <color theme="1"/>
+      <family val="2"/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
+      <color theme="10"/>
+      <family val="2"/>
       <sz val="11"/>
-      <color theme="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
+      <color theme="1"/>
       <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
@@ -766,7 +768,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1096,15 +1098,15 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="9.140625" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
@@ -1114,8 +1116,8 @@
     <col min="8" max="8" width="71.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="15" customHeight="1"/>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1">
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" ht="15.75" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
+    <row r="5" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -1159,7 +1161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
+    <row r="6" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -1177,7 +1179,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
+    <row r="7" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
@@ -1195,351 +1197,355 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="A8" s="2"/>
+    <row r="8" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
-      <c r="A9" s="2"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="29.25" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" ht="29.25" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="29.25" customHeight="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" ht="29.25" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1548,781 +1554,781 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H5" r:id="rId1"/>
+    <hyperlink ref="H11" r:id="rId2"/>
+    <hyperlink ref="H24" r:id="rId3"/>
+    <hyperlink ref="H28" r:id="rId4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="9.140625" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="2" width="59.5703125" customWidth="1"/>
     <col min="3" max="3" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="42.75" customHeight="1">
+    <row r="2" ht="42.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" ht="42.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15">
-      <c r="B5" t="s">
+    <row r="23" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
-      <c r="B6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15">
-      <c r="B7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15">
-      <c r="B8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15">
-      <c r="B9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15">
-      <c r="B10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15">
-      <c r="B11" t="s">
+    <row r="24" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
-      <c r="B12" t="s">
+    <row r="49" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C55" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="56" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="57" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="58" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="60" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15">
-      <c r="B13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15">
-      <c r="B14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15">
-      <c r="B15" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15">
-      <c r="B16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15">
-      <c r="B17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15">
-      <c r="B18" t="s">
+    <row r="61" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="65" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="66" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="69" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="71" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="72" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="73" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="75" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="77" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="78" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="82" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="83" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="84" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="85" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="86" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="87" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="88" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="89" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="90" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="91" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="92" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="93" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="94" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="95" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="96" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="42.75" customHeight="1">
-      <c r="A21" s="5" t="s">
+    <row r="97" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
         <v>143</v>
       </c>
-      <c r="B21" t="s">
-        <v>144</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15">
-      <c r="B22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15">
-      <c r="B23" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15">
-      <c r="B24" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15">
-      <c r="B25" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15">
-      <c r="B26" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15">
-      <c r="B27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15">
-      <c r="B28" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15">
-      <c r="B29" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15">
-      <c r="B30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15">
-      <c r="B31" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15">
-      <c r="B32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15">
-      <c r="B33" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15">
-      <c r="B34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15">
-      <c r="B35" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15">
-      <c r="B36" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15">
-      <c r="B37" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15">
-      <c r="B38" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15">
-      <c r="B39" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15">
-      <c r="B40" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15">
-      <c r="B41" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15">
-      <c r="B42" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="15">
-      <c r="B43" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="15">
-      <c r="B44" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15">
-      <c r="A47" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B47" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="15">
-      <c r="B48" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" ht="15">
-      <c r="B49" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="15">
-      <c r="B50" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" ht="15">
-      <c r="B51" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" ht="15">
-      <c r="B52" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" ht="15">
-      <c r="B53" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" ht="15">
-      <c r="B54" t="s">
-        <v>166</v>
-      </c>
-      <c r="C54" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" ht="15">
-      <c r="B55" t="s">
-        <v>168</v>
-      </c>
-      <c r="C55" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" ht="15">
-      <c r="B56" t="s">
-        <v>170</v>
-      </c>
-      <c r="C56" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" ht="15">
-      <c r="B57" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" ht="15">
-      <c r="B58" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" ht="15">
-      <c r="B59" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" ht="15">
-      <c r="B60" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" ht="15">
-      <c r="B61" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" ht="15">
-      <c r="B62" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" ht="15">
-      <c r="B63" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" ht="15">
-      <c r="B64" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" ht="15">
-      <c r="B65" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" ht="15">
-      <c r="B66" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" ht="15">
-      <c r="B67" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" ht="15">
-      <c r="B68" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" ht="15">
-      <c r="B69" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" ht="15">
-      <c r="B70" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" ht="15">
-      <c r="B71" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" ht="15">
-      <c r="B72" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" ht="15">
-      <c r="B73" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" ht="15">
-      <c r="B74" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" ht="15">
-      <c r="B75" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" ht="15">
-      <c r="B76" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" ht="15">
-      <c r="B77" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" ht="15">
-      <c r="B78" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" ht="15">
-      <c r="B79" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" ht="15">
-      <c r="B80" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" ht="15">
-      <c r="B81" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" ht="15">
-      <c r="B82" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" ht="15">
-      <c r="B83" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2" ht="15">
-      <c r="B84" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" ht="15">
-      <c r="B85" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" ht="15">
-      <c r="B86" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" ht="15">
-      <c r="B87" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" ht="15">
-      <c r="B88" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" ht="15">
-      <c r="B89" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" ht="15">
-      <c r="B90" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" ht="15">
-      <c r="B91" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" ht="15">
-      <c r="B92" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2" ht="15">
-      <c r="B93" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2" ht="15">
-      <c r="B94" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" ht="15">
-      <c r="B95" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" ht="15">
-      <c r="B96" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" ht="15">
-      <c r="B97" t="s">
-        <v>142</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: work for Onur
</commit_message>
<xml_diff>
--- a/.design/Join_Projektuebersicht.xlsx
+++ b/.design/Join_Projektuebersicht.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="204">
   <si>
     <t>Name/Namen</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Registrierungsseite für neue Nutzer.</t>
+  </si>
+  <si>
+    <t>Onur</t>
   </si>
   <si>
     <t>summary.html</t>
@@ -1238,41 +1241,43 @@
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" ht="29.25" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1280,17 +1285,17 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1298,17 +1303,17 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1316,35 +1321,35 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1352,17 +1357,17 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1371,16 +1376,16 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1389,16 +1394,16 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1406,17 +1411,17 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1424,17 +1429,17 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1443,16 +1448,16 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" ht="29.25" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1461,34 +1466,34 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1496,17 +1501,17 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1514,17 +1519,17 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1532,17 +1537,17 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1554,13 +1559,13 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1569,16 +1574,16 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1587,16 +1592,16 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1605,16 +1610,16 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1623,34 +1628,34 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1658,17 +1663,17 @@
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1676,17 +1681,17 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1694,17 +1699,17 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1712,17 +1717,17 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1730,17 +1735,17 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1748,17 +1753,17 @@
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1766,17 +1771,17 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1784,17 +1789,17 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1802,17 +1807,17 @@
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1843,489 +1848,489 @@
   <sheetData>
     <row r="2" ht="42.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" ht="42.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B47" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C54" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C55" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C56" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="83" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="84" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="87" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="89" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="90" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="91" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="92" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="93" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="94" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="95" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: work for Thomas
</commit_message>
<xml_diff>
--- a/.design/Join_Projektuebersicht.xlsx
+++ b/.design/Join_Projektuebersicht.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="205">
   <si>
     <t>Name/Namen</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Kanban‑Board mit Spalten (To Do, In Progress, Await Feedback, Done).geeksforgeeks​</t>
+  </si>
+  <si>
+    <t>Thomas</t>
   </si>
   <si>
     <t>add-task.html</t>
@@ -1281,39 +1284,43 @@
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1321,35 +1328,35 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1357,17 +1364,17 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1376,16 +1383,16 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1394,16 +1401,16 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1411,17 +1418,17 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1429,17 +1436,17 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1448,16 +1455,16 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" ht="29.25" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1466,34 +1473,34 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1501,17 +1508,17 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1519,17 +1526,17 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1537,17 +1544,17 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1559,13 +1566,13 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1574,16 +1581,16 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1592,16 +1599,16 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1610,16 +1617,16 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1628,34 +1635,34 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1663,17 +1670,17 @@
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1681,17 +1688,17 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1699,17 +1706,17 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1717,17 +1724,17 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1735,17 +1742,17 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1753,17 +1760,17 @@
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1771,17 +1778,17 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1789,17 +1796,17 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1807,17 +1814,17 @@
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1848,489 +1855,489 @@
   <sheetData>
     <row r="2" ht="42.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" ht="42.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B47" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C54" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C55" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C56" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="81" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="87" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="89" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="92" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="93" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="94" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="95" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="96" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="97" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: nav-bar as single component for all pages
</commit_message>
<xml_diff>
--- a/.design/Join_Projektuebersicht.xlsx
+++ b/.design/Join_Projektuebersicht.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5449C2C-79B9-46EC-BBA7-22714E7B1E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="2" name="Folder and File" state="visible" r:id="rId4"/>
-    <sheet sheetId="3" name="DummyData" state="visible" r:id="rId5"/>
+    <sheet name="Folder and File" sheetId="2" r:id="rId1"/>
+    <sheet name="DummyData" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="212">
   <si>
     <t>Name/Namen</t>
   </si>
@@ -403,10 +404,10 @@
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
         <color theme="1"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (für Login/Registrierung bzw. Profil)</t>
     </r>
@@ -415,7 +416,7 @@
     <t>// users (Collection)</t>
   </si>
   <si>
-    <t xml:space="preserve">Kann sich einloggen
+    <t>Kann sich einloggen
 Sieht Summary, Board, Contacts
 Erstellt, bearbeitet und verschiebt Tasks</t>
   </si>
@@ -473,10 +474,10 @@
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
         <color theme="1"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (für Zuweisungen)</t>
     </r>
@@ -485,7 +486,7 @@
     <t>// contacts (Collection)</t>
   </si>
   <si>
-    <t xml:space="preserve">Können Tasks zugewiesen bekommen
+    <t>Können Tasks zugewiesen bekommen
 Müssen keinen Login haben
 Dienen rein der Organisation</t>
   </si>
@@ -537,10 +538,10 @@
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
         <color theme="1"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (fürs Board)</t>
     </r>
@@ -667,43 +668,64 @@
   </si>
   <si>
     <t xml:space="preserve">    "createdAt": "2026-01-01T12:00:00.000Z"</t>
+  </si>
+  <si>
+    <t>components</t>
+  </si>
+  <si>
+    <t>join/pages/components/nav-bar.html</t>
+  </si>
+  <si>
+    <t>nav-bar.html</t>
+  </si>
+  <si>
+    <t>Seitenmenue Links</t>
+  </si>
+  <si>
+    <t>components.js</t>
+  </si>
+  <si>
+    <t>join/js/components.js</t>
+  </si>
+  <si>
+    <t>Auf mehreren Seiten verwendete Objekte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color theme="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
-      <sz val="10"/>
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
@@ -774,7 +796,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1104,17 +1126,18 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H41"/>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:H47"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="9.140625" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="38.85546875" customWidth="1"/>
@@ -1122,8 +1145,8 @@
     <col min="8" max="8" width="71.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" ht="15.75" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1149,7 +1172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -1167,7 +1190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -1185,7 +1208,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
@@ -1203,7 +1226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1223,7 +1246,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1243,7 +1266,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1263,7 +1286,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" ht="29.25" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1283,7 +1306,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -1303,7 +1326,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -1323,7 +1346,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1341,519 +1364,599 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3" t="s">
+        <v>205</v>
+      </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>207</v>
+      </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="D18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
-        <v>62</v>
-      </c>
+      <c r="D21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" ht="29.25" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="D22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="F23" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="F24" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="C25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="3" t="s">
-        <v>15</v>
+      <c r="D27" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="D28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H28" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2" t="s">
-        <v>90</v>
-      </c>
+      <c r="D30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="F32" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="F33" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="F34" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="C37" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>101</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>101</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>101</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>101</v>
       </c>
       <c r="H41" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>126</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1"/>
-    <hyperlink ref="H11" r:id="rId2"/>
-    <hyperlink ref="H24" r:id="rId3"/>
-    <hyperlink ref="H28" r:id="rId4"/>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H26" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H31" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:C97"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="9.140625" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="2" width="59.5703125" customWidth="1"/>
     <col min="3" max="3" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="42.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>127</v>
       </c>
@@ -1864,37 +1967,37 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>136</v>
       </c>
@@ -1902,52 +2005,52 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="11" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="16" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="18" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="21" ht="42.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>146</v>
       </c>
@@ -1958,122 +2061,122 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="23" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="25" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="26" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="27" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="29" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="30" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="31" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="32" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="33" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="34" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="35" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="36" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="37" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="38" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="39" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="40" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="41" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="42" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="44" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="47" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>163</v>
       </c>
@@ -2081,37 +2184,37 @@
         <v>164</v>
       </c>
     </row>
-    <row r="48" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="49" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="50" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="51" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="52" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="53" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="54" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>169</v>
       </c>
@@ -2119,7 +2222,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="55" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>171</v>
       </c>
@@ -2127,7 +2230,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="56" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>173</v>
       </c>
@@ -2135,212 +2238,212 @@
         <v>174</v>
       </c>
     </row>
-    <row r="57" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="58" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="59" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="60" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="61" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="62" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="63" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="64" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="65" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="66" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="67" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="68" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="69" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="70" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="71" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="72" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="73" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="74" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="75" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="76" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="77" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="78" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="79" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="80" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="81" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="82" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="83" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="84" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="85" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="86" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="87" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="88" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="89" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="90" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="91" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="92" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="93" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="94" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="95" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="96" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="97" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>145</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: createt new folders and same dummyData for all
</commit_message>
<xml_diff>
--- a/.design/Join_Projektuebersicht.xlsx
+++ b/.design/Join_Projektuebersicht.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5449C2C-79B9-46EC-BBA7-22714E7B1E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062CC03E-02DD-4B9E-A570-06FFD8922C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folder and File" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="213">
   <si>
     <t>Name/Namen</t>
   </si>
@@ -204,22 +204,7 @@
     <t>Beispiel‑Daten für Entwicklung und Tests.</t>
   </si>
   <si>
-    <t>sample-tasks.json</t>
-  </si>
-  <si>
-    <t>join/assets/dummy-data/sample-tasks.json</t>
-  </si>
-  <si>
-    <t>Datei (JSON)</t>
-  </si>
-  <si>
     <t>Beispiel‑Tasks für erste Tests.</t>
-  </si>
-  <si>
-    <t>sample-contacts.json</t>
-  </si>
-  <si>
-    <t>join/assets/dummy-data/sample-contacts.json</t>
   </si>
   <si>
     <t>Beispiel‑Kontakte für erste Tests.</t>
@@ -690,18 +675,42 @@
   <si>
     <t>Auf mehreren Seiten verwendete Objekte</t>
   </si>
+  <si>
+    <t>sample-tasks.js</t>
+  </si>
+  <si>
+    <t>sample-contacts.js</t>
+  </si>
+  <si>
+    <t>sample-users.js</t>
+  </si>
+  <si>
+    <t>join/assets/dummy-data/sample-contacts.js</t>
+  </si>
+  <si>
+    <t>join/assets/dummy-data/sample-tasks.js</t>
+  </si>
+  <si>
+    <t>Beispiel-Users für die ersten Tests</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -776,23 +785,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1128,13 +1140,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:H47"/>
+  <dimension ref="A3:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
@@ -1145,8 +1157,8 @@
     <col min="8" max="8" width="71.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1"/>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -1190,7 +1202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -1208,7 +1220,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
@@ -1226,7 +1238,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1246,7 +1258,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1266,7 +1278,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1286,7 +1298,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="29.25" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1306,7 +1318,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -1326,7 +1338,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -1346,7 +1358,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1364,12 +1376,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1378,25 +1390,25 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3" t="s">
@@ -1414,7 +1426,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1432,7 +1444,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1450,7 +1462,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1468,7 +1480,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1486,7 +1498,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1504,225 +1516,233 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="28.5">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" ht="29.25" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>67</v>
+      <c r="E24" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="29.25" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2" t="s">
-        <v>70</v>
+      <c r="E25" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="C26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="27" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="D31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1732,210 +1752,220 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15" customHeight="1">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="C38" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>209</v>
+        <v>98</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>210</v>
+        <v>99</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>106</v>
+        <v>204</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>107</v>
+        <v>205</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" customHeight="1">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15" customHeight="1">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="H11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H26" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H31" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H27" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H32" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1949,498 +1979,498 @@
       <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="2" width="59.5703125" customWidth="1"/>
     <col min="3" max="3" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="42.75" customHeight="1">
       <c r="A2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1">
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1">
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1">
+      <c r="B5" t="s">
         <v>127</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1">
+      <c r="B6" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="6" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1">
+      <c r="B7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="8" spans="1:3" ht="15" customHeight="1">
+      <c r="B8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="9" spans="1:3" ht="15" customHeight="1">
+      <c r="B9" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C9" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="10" spans="1:3" ht="15" customHeight="1">
+      <c r="B10" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="11" spans="1:3" ht="15" customHeight="1">
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1">
+      <c r="B12" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="13" spans="1:3" ht="15" customHeight="1">
+      <c r="B13" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="14" spans="1:3" ht="15" customHeight="1">
+      <c r="B14" t="s">
         <v>136</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1">
+      <c r="B15" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="16" spans="1:3" ht="15" customHeight="1">
+      <c r="B16" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="17" spans="1:3" ht="15" customHeight="1">
+      <c r="B17" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="18" spans="1:3" ht="15" customHeight="1">
+      <c r="B18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="21" spans="1:3" ht="42.75" customHeight="1">
+      <c r="A21" s="5" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B21" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C21" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="22" spans="1:3" ht="15" customHeight="1">
+      <c r="B22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1">
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" customHeight="1">
+      <c r="B24" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="25" spans="1:3" ht="15" customHeight="1">
+      <c r="B25" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+    <row r="26" spans="1:3" ht="15" customHeight="1">
+      <c r="B26" t="s">
         <v>146</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1">
+      <c r="B27" t="s">
         <v>147</v>
       </c>
-      <c r="C21" s="6" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="15" customHeight="1">
+      <c r="B28" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="29" spans="1:3" ht="15" customHeight="1">
+      <c r="B29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" customHeight="1">
+      <c r="B30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" customHeight="1">
+      <c r="B31" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="32" spans="1:3" ht="15" customHeight="1">
+      <c r="B32" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="33" spans="1:2" ht="15" customHeight="1">
+      <c r="B33" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="34" spans="1:2" ht="15" customHeight="1">
+      <c r="B34" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="35" spans="1:2" ht="15" customHeight="1">
+      <c r="B35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" customHeight="1">
+      <c r="B36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" customHeight="1">
+      <c r="B37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15" customHeight="1">
+      <c r="B38" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="39" spans="1:2" ht="15" customHeight="1">
+      <c r="B39" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="40" spans="1:2" ht="15" customHeight="1">
+      <c r="B40" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="41" spans="1:2" ht="15" customHeight="1">
+      <c r="B41" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="42" spans="1:2" ht="15" customHeight="1">
+      <c r="B42" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="43" spans="1:2" ht="15" customHeight="1">
+      <c r="B43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15" customHeight="1">
+      <c r="B44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" customHeight="1">
+      <c r="A47" s="5" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="B47" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="48" spans="1:2" ht="15" customHeight="1">
+      <c r="B48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="15" customHeight="1">
+      <c r="B49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="15" customHeight="1">
+      <c r="B50" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="51" spans="2:3" ht="15" customHeight="1">
+      <c r="B51" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="52" spans="2:3" ht="15" customHeight="1">
+      <c r="B52" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+    <row r="53" spans="2:3" ht="15" customHeight="1">
+      <c r="B53" t="s">
         <v>163</v>
       </c>
-      <c r="B47" t="s">
+    </row>
+    <row r="54" spans="2:3" ht="15" customHeight="1">
+      <c r="B54" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="C54" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="55" spans="2:3" ht="15" customHeight="1">
+      <c r="B55" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="52" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+      <c r="C55" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="56" spans="2:3" ht="15" customHeight="1">
+      <c r="B56" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="54" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="C56" t="s">
         <v>169</v>
       </c>
-      <c r="C54" t="s">
+    </row>
+    <row r="57" spans="2:3" ht="15" customHeight="1">
+      <c r="B57" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="58" spans="2:3" ht="15" customHeight="1">
+      <c r="B58" t="s">
         <v>171</v>
       </c>
-      <c r="C55" t="s">
+    </row>
+    <row r="59" spans="2:3" ht="15" customHeight="1">
+      <c r="B59" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="60" spans="2:3" ht="15" customHeight="1">
+      <c r="B60" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" ht="15" customHeight="1">
+      <c r="B61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" ht="15" customHeight="1">
+      <c r="B62" t="s">
         <v>173</v>
       </c>
-      <c r="C56" t="s">
+    </row>
+    <row r="63" spans="2:3" ht="15" customHeight="1">
+      <c r="B63" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="57" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="64" spans="2:3" ht="15" customHeight="1">
+      <c r="B64" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="65" spans="2:2" ht="15" customHeight="1">
+      <c r="B65" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="66" spans="2:2" ht="15" customHeight="1">
+      <c r="B66" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="60" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="67" spans="2:2" ht="15" customHeight="1">
+      <c r="B67" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="68" spans="2:2" ht="15" customHeight="1">
+      <c r="B68" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="64" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="69" spans="2:2" ht="15" customHeight="1">
+      <c r="B69" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="70" spans="2:2" ht="15" customHeight="1">
+      <c r="B70" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" ht="15" customHeight="1">
+      <c r="B71" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="66" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="72" spans="2:2" ht="15" customHeight="1">
+      <c r="B72" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" ht="15" customHeight="1">
+      <c r="B73" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" ht="15" customHeight="1">
+      <c r="B74" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+    <row r="75" spans="2:2" ht="15" customHeight="1">
+      <c r="B75" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="68" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="76" spans="2:2" ht="15" customHeight="1">
+      <c r="B76" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="69" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+    <row r="77" spans="2:2" ht="15" customHeight="1">
+      <c r="B77" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" ht="15" customHeight="1">
+      <c r="B78" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
+    <row r="79" spans="2:2" ht="15" customHeight="1">
+      <c r="B79" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="80" spans="2:2" ht="15" customHeight="1">
+      <c r="B80" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="75" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="81" spans="2:2" ht="15" customHeight="1">
+      <c r="B81" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="76" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="82" spans="2:2" ht="15" customHeight="1">
+      <c r="B82" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="77" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+    <row r="83" spans="2:2" ht="15" customHeight="1">
+      <c r="B83" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+    <row r="84" spans="2:2" ht="15" customHeight="1">
+      <c r="B84" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" ht="15" customHeight="1">
+      <c r="B85" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" ht="15" customHeight="1">
+      <c r="B86" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="80" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
+    <row r="87" spans="2:2" ht="15" customHeight="1">
+      <c r="B87" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+    <row r="88" spans="2:2" ht="15" customHeight="1">
+      <c r="B88" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+    <row r="89" spans="2:2" ht="15" customHeight="1">
+      <c r="B89" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+    <row r="90" spans="2:2" ht="15" customHeight="1">
+      <c r="B90" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+    <row r="91" spans="2:2" ht="15" customHeight="1">
+      <c r="B91" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="87" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
+    <row r="92" spans="2:2" ht="15" customHeight="1">
+      <c r="B92" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="88" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+    <row r="93" spans="2:2" ht="15" customHeight="1">
+      <c r="B93" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="89" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+    <row r="94" spans="2:2" ht="15" customHeight="1">
+      <c r="B94" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" ht="15" customHeight="1">
+      <c r="B95" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="90" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" ht="15" customHeight="1">
       <c r="B96" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" ht="15" customHeight="1">
       <c r="B97" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>